<commit_message>
Version 0.5 - Weekly Update, updated LCA
</commit_message>
<xml_diff>
--- a/content/background_data_decision_tree.xlsx
+++ b/content/background_data_decision_tree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://skznet-my.sharepoint.com/personal/j_werner_skz_de/Documents/PlastIQ/Bearbeitung/AP3_Generische Modelle/Entwicklung Entscheidungsschema/02_Hintergrunddaten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="486" documentId="8_{03825F57-9271-4F19-AB31-225796C02C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{276AD160-D35D-4CE1-990C-23A52A124C5C}"/>
+  <xr:revisionPtr revIDLastSave="510" documentId="8_{03825F57-9271-4F19-AB31-225796C02C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1FC9750-9AA7-4A4C-8523-283C18A3B6CF}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-2955" windowWidth="18240" windowHeight="28440" firstSheet="2" activeTab="5" xr2:uid="{9E0EC3E4-013A-49B8-ADD7-0C11DDD362E4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="5" xr2:uid="{9E0EC3E4-013A-49B8-ADD7-0C11DDD362E4}"/>
   </bookViews>
   <sheets>
     <sheet name="list_material" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="169">
   <si>
     <t>ABS</t>
   </si>
@@ -522,6 +522,36 @@
   <si>
     <t xml:space="preserve">PS, </t>
   </si>
+  <si>
+    <t>electric_DE_mix</t>
+  </si>
+  <si>
+    <t>heat_DE_mix</t>
+  </si>
+  <si>
+    <t>electric_DE_wind</t>
+  </si>
+  <si>
+    <t>electric_DE_medium_voltage</t>
+  </si>
+  <si>
+    <t>electric_AT_medium_voltage</t>
+  </si>
+  <si>
+    <t>electric_CH_medium_voltage</t>
+  </si>
+  <si>
+    <t>electric_DE_green</t>
+  </si>
+  <si>
+    <t>electric_DE_water</t>
+  </si>
+  <si>
+    <t>electric_DE_solar</t>
+  </si>
+  <si>
+    <t>heat_DE_natural_gas</t>
+  </si>
 </sst>
 </file>
 
@@ -587,11 +617,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1047,17 +1077,17 @@
       <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1080,8 +1110,8 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
@@ -1100,8 +1130,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
@@ -1120,8 +1150,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
@@ -1140,7 +1170,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1160,8 +1190,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C6" t="s">
@@ -1180,8 +1210,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
@@ -1200,7 +1230,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1217,8 +1247,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
@@ -1237,8 +1267,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C10" t="s">
@@ -1257,8 +1287,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
@@ -1277,7 +1307,7 @@
         <v>38.07</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1290,11 +1320,11 @@
       <c r="E12" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>38.07</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1307,12 +1337,12 @@
       <c r="E13" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>38.07</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C14" t="s">
@@ -1328,8 +1358,8 @@
         <v>27.36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
@@ -1348,8 +1378,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
@@ -1368,8 +1398,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C17" t="s">
@@ -1385,7 +1415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1399,8 +1429,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C19" t="s">
@@ -1413,8 +1443,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C20" t="s">
@@ -1430,7 +1460,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1447,7 +1477,7 @@
         <v>27.36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1461,8 +1491,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C23" t="s">
@@ -1478,8 +1508,8 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C24" t="s">
@@ -1495,7 +1525,7 @@
         <v>23.04</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1515,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1532,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1549,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1569,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -1589,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -1606,7 +1636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -1623,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -1643,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -1660,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -1691,12 +1721,12 @@
       <selection activeCell="B2" sqref="B2:AH34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1833,7 +1863,7 @@
         <v>Zink</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="str">
         <f>list_material!A2</f>
         <v>PE-LD</v>
@@ -1938,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str">
         <f>list_material!A3</f>
         <v>PE-LLD</v>
@@ -2043,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <f>list_material!A4</f>
         <v>PE-HD</v>
@@ -2148,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="str">
         <f>list_material!A5</f>
         <v>PE-MD</v>
@@ -2253,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="str">
         <f>list_material!A6</f>
         <v>PP</v>
@@ -2358,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="str">
         <f>list_material!A7</f>
         <v>PS</v>
@@ -2463,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="str">
         <f>list_material!A8</f>
         <v>PS-E/XPS</v>
@@ -2568,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="str">
         <f>list_material!A9</f>
         <v>PVC-U</v>
@@ -2673,7 +2703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="str">
         <f>list_material!A10</f>
         <v>PVC-P</v>
@@ -2778,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="str">
         <f>list_material!A11</f>
         <v>ABS</v>
@@ -2883,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="str">
         <f>list_material!A12</f>
         <v>ASA</v>
@@ -2988,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="str">
         <f>list_material!A13</f>
         <v>SAN</v>
@@ -3093,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="str">
         <f>list_material!A14</f>
         <v>PMMA</v>
@@ -3198,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="str">
         <f>list_material!A15</f>
         <v>PA</v>
@@ -3303,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="str">
         <f>list_material!A16</f>
         <v>PET</v>
@@ -3408,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="str">
         <f>list_material!A17</f>
         <v>POM</v>
@@ -3513,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="str">
         <f>list_material!A18</f>
         <v>PBT</v>
@@ -3618,7 +3648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="str">
         <f>list_material!A19</f>
         <v>PEEK</v>
@@ -3723,7 +3753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="str">
         <f>list_material!A20</f>
         <v>PC</v>
@@ -3828,7 +3858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f>list_material!A21</f>
         <v>PUR</v>
@@ -3933,7 +3963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="str">
         <f>list_material!A22</f>
         <v>Thermoplaste</v>
@@ -4038,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="str">
         <f>list_material!A23</f>
         <v>Elastomere</v>
@@ -4143,7 +4173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="str">
         <f>list_material!A24</f>
         <v>Duromere</v>
@@ -4248,7 +4278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="str">
         <f>list_material!A25</f>
         <v>Aluminium</v>
@@ -4353,7 +4383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="str">
         <f>list_material!A26</f>
         <v>Blei</v>
@@ -4458,7 +4488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="str">
         <f>list_material!A27</f>
         <v>Chrom</v>
@@ -4563,7 +4593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="str">
         <f>list_material!A28</f>
         <v>Eisen</v>
@@ -4668,7 +4698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="str">
         <f>list_material!A29</f>
         <v>Kupfer</v>
@@ -4773,7 +4803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="str">
         <f>list_material!A30</f>
         <v>Magnesium</v>
@@ -4878,7 +4908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="str">
         <f>list_material!A31</f>
         <v>Nickel</v>
@@ -4983,7 +5013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="str">
         <f>list_material!A32</f>
         <v>Stahl</v>
@@ -5088,7 +5118,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="str">
         <f>list_material!A33</f>
         <v>Titan</v>
@@ -5193,7 +5223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="str">
         <f>list_material!A34</f>
         <v>Zink</v>
@@ -5311,9 +5341,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -5450,7 +5480,7 @@
         <v>Zink</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="str">
         <f>list_material!A2</f>
         <v>PE-LD</v>
@@ -5555,7 +5585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str">
         <f>list_material!A3</f>
         <v>PE-LLD</v>
@@ -5660,7 +5690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <f>list_material!A4</f>
         <v>PE-HD</v>
@@ -5765,7 +5795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="str">
         <f>list_material!A5</f>
         <v>PE-MD</v>
@@ -5870,7 +5900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="str">
         <f>list_material!A6</f>
         <v>PP</v>
@@ -5975,7 +6005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="str">
         <f>list_material!A7</f>
         <v>PS</v>
@@ -6080,7 +6110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="str">
         <f>list_material!A8</f>
         <v>PS-E/XPS</v>
@@ -6185,7 +6215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="str">
         <f>list_material!A9</f>
         <v>PVC-U</v>
@@ -6290,7 +6320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="str">
         <f>list_material!A10</f>
         <v>PVC-P</v>
@@ -6395,7 +6425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="str">
         <f>list_material!A11</f>
         <v>ABS</v>
@@ -6500,7 +6530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="str">
         <f>list_material!A12</f>
         <v>ASA</v>
@@ -6605,7 +6635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="str">
         <f>list_material!A13</f>
         <v>SAN</v>
@@ -6710,7 +6740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="str">
         <f>list_material!A14</f>
         <v>PMMA</v>
@@ -6815,7 +6845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="str">
         <f>list_material!A15</f>
         <v>PA</v>
@@ -6920,7 +6950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="str">
         <f>list_material!A16</f>
         <v>PET</v>
@@ -7025,7 +7055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="str">
         <f>list_material!A17</f>
         <v>POM</v>
@@ -7130,7 +7160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="str">
         <f>list_material!A18</f>
         <v>PBT</v>
@@ -7235,7 +7265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="str">
         <f>list_material!A19</f>
         <v>PEEK</v>
@@ -7340,7 +7370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="str">
         <f>list_material!A20</f>
         <v>PC</v>
@@ -7445,7 +7475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f>list_material!A21</f>
         <v>PUR</v>
@@ -7550,7 +7580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="str">
         <f>list_material!A22</f>
         <v>Thermoplaste</v>
@@ -7655,7 +7685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="str">
         <f>list_material!A23</f>
         <v>Elastomere</v>
@@ -7760,7 +7790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="str">
         <f>list_material!A24</f>
         <v>Duromere</v>
@@ -7865,7 +7895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="str">
         <f>list_material!A25</f>
         <v>Aluminium</v>
@@ -7970,7 +8000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="str">
         <f>list_material!A26</f>
         <v>Blei</v>
@@ -8075,7 +8105,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="str">
         <f>list_material!A27</f>
         <v>Chrom</v>
@@ -8180,7 +8210,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="str">
         <f>list_material!A28</f>
         <v>Eisen</v>
@@ -8285,7 +8315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="str">
         <f>list_material!A29</f>
         <v>Kupfer</v>
@@ -8390,7 +8420,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="str">
         <f>list_material!A30</f>
         <v>Magnesium</v>
@@ -8495,7 +8525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="str">
         <f>list_material!A31</f>
         <v>Nickel</v>
@@ -8600,7 +8630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="str">
         <f>list_material!A32</f>
         <v>Stahl</v>
@@ -8705,7 +8735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="str">
         <f>list_material!A33</f>
         <v>Titan</v>
@@ -8810,7 +8840,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="str">
         <f>list_material!A34</f>
         <v>Zink</v>
@@ -8928,9 +8958,9 @@
       <selection activeCell="A2" sqref="A2:A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -9067,7 +9097,7 @@
         <v>Zink</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="str">
         <f>list_material!A2</f>
         <v>PE-LD</v>
@@ -9172,7 +9202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str">
         <f>list_material!A3</f>
         <v>PE-LLD</v>
@@ -9277,7 +9307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <f>list_material!A4</f>
         <v>PE-HD</v>
@@ -9382,7 +9412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="str">
         <f>list_material!A5</f>
         <v>PE-MD</v>
@@ -9487,7 +9517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="str">
         <f>list_material!A6</f>
         <v>PP</v>
@@ -9592,7 +9622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="str">
         <f>list_material!A7</f>
         <v>PS</v>
@@ -9697,7 +9727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="str">
         <f>list_material!A8</f>
         <v>PS-E/XPS</v>
@@ -9802,7 +9832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="str">
         <f>list_material!A9</f>
         <v>PVC-U</v>
@@ -9907,7 +9937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="str">
         <f>list_material!A10</f>
         <v>PVC-P</v>
@@ -10012,7 +10042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="str">
         <f>list_material!A11</f>
         <v>ABS</v>
@@ -10117,7 +10147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="str">
         <f>list_material!A12</f>
         <v>ASA</v>
@@ -10222,7 +10252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="str">
         <f>list_material!A13</f>
         <v>SAN</v>
@@ -10327,7 +10357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="str">
         <f>list_material!A14</f>
         <v>PMMA</v>
@@ -10432,7 +10462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="str">
         <f>list_material!A15</f>
         <v>PA</v>
@@ -10537,7 +10567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="str">
         <f>list_material!A16</f>
         <v>PET</v>
@@ -10642,7 +10672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="str">
         <f>list_material!A17</f>
         <v>POM</v>
@@ -10747,7 +10777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="str">
         <f>list_material!A18</f>
         <v>PBT</v>
@@ -10852,7 +10882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="str">
         <f>list_material!A19</f>
         <v>PEEK</v>
@@ -10957,7 +10987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="str">
         <f>list_material!A20</f>
         <v>PC</v>
@@ -11062,7 +11092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f>list_material!A21</f>
         <v>PUR</v>
@@ -11167,7 +11197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="str">
         <f>list_material!A22</f>
         <v>Thermoplaste</v>
@@ -11272,7 +11302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="str">
         <f>list_material!A23</f>
         <v>Elastomere</v>
@@ -11377,7 +11407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="str">
         <f>list_material!A24</f>
         <v>Duromere</v>
@@ -11482,7 +11512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="str">
         <f>list_material!A25</f>
         <v>Aluminium</v>
@@ -11587,7 +11617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="str">
         <f>list_material!A26</f>
         <v>Blei</v>
@@ -11692,7 +11722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="str">
         <f>list_material!A27</f>
         <v>Chrom</v>
@@ -11797,7 +11827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="str">
         <f>list_material!A28</f>
         <v>Eisen</v>
@@ -11902,7 +11932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="str">
         <f>list_material!A29</f>
         <v>Kupfer</v>
@@ -12007,7 +12037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="str">
         <f>list_material!A30</f>
         <v>Magnesium</v>
@@ -12112,7 +12142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="str">
         <f>list_material!A31</f>
         <v>Nickel</v>
@@ -12217,7 +12247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="str">
         <f>list_material!A32</f>
         <v>Stahl</v>
@@ -12322,7 +12352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="str">
         <f>list_material!A33</f>
         <v>Titan</v>
@@ -12427,7 +12457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="str">
         <f>list_material!A34</f>
         <v>Zink</v>
@@ -12545,9 +12575,9 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -12684,7 +12714,7 @@
         <v>Zink</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="str">
         <f>list_material!A2</f>
         <v>PE-LD</v>
@@ -12789,7 +12819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str">
         <f>list_material!A3</f>
         <v>PE-LLD</v>
@@ -12894,7 +12924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
         <f>list_material!A4</f>
         <v>PE-HD</v>
@@ -12999,7 +13029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="str">
         <f>list_material!A5</f>
         <v>PE-MD</v>
@@ -13104,7 +13134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="str">
         <f>list_material!A6</f>
         <v>PP</v>
@@ -13209,7 +13239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="str">
         <f>list_material!A7</f>
         <v>PS</v>
@@ -13314,7 +13344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="str">
         <f>list_material!A8</f>
         <v>PS-E/XPS</v>
@@ -13419,7 +13449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="str">
         <f>list_material!A9</f>
         <v>PVC-U</v>
@@ -13524,7 +13554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="str">
         <f>list_material!A10</f>
         <v>PVC-P</v>
@@ -13629,7 +13659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="str">
         <f>list_material!A11</f>
         <v>ABS</v>
@@ -13734,7 +13764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="str">
         <f>list_material!A12</f>
         <v>ASA</v>
@@ -13839,7 +13869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="str">
         <f>list_material!A13</f>
         <v>SAN</v>
@@ -13944,7 +13974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="str">
         <f>list_material!A14</f>
         <v>PMMA</v>
@@ -14049,7 +14079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="str">
         <f>list_material!A15</f>
         <v>PA</v>
@@ -14154,7 +14184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="str">
         <f>list_material!A16</f>
         <v>PET</v>
@@ -14259,7 +14289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="str">
         <f>list_material!A17</f>
         <v>POM</v>
@@ -14364,7 +14394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="str">
         <f>list_material!A18</f>
         <v>PBT</v>
@@ -14469,7 +14499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="str">
         <f>list_material!A19</f>
         <v>PEEK</v>
@@ -14574,7 +14604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="str">
         <f>list_material!A20</f>
         <v>PC</v>
@@ -14679,7 +14709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
         <f>list_material!A21</f>
         <v>PUR</v>
@@ -14784,7 +14814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="str">
         <f>list_material!A22</f>
         <v>Thermoplaste</v>
@@ -14889,7 +14919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="str">
         <f>list_material!A23</f>
         <v>Elastomere</v>
@@ -14994,7 +15024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="str">
         <f>list_material!A24</f>
         <v>Duromere</v>
@@ -15099,7 +15129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="str">
         <f>list_material!A25</f>
         <v>Aluminium</v>
@@ -15204,7 +15234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="str">
         <f>list_material!A26</f>
         <v>Blei</v>
@@ -15309,7 +15339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="str">
         <f>list_material!A27</f>
         <v>Chrom</v>
@@ -15414,7 +15444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="str">
         <f>list_material!A28</f>
         <v>Eisen</v>
@@ -15519,7 +15549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="str">
         <f>list_material!A29</f>
         <v>Kupfer</v>
@@ -15624,7 +15654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="str">
         <f>list_material!A30</f>
         <v>Magnesium</v>
@@ -15729,7 +15759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="str">
         <f>list_material!A31</f>
         <v>Nickel</v>
@@ -15834,7 +15864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="str">
         <f>list_material!A32</f>
         <v>Stahl</v>
@@ -15939,7 +15969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="str">
         <f>list_material!A33</f>
         <v>Titan</v>
@@ -16044,7 +16074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="str">
         <f>list_material!A34</f>
         <v>Zink</v>
@@ -16158,17 +16188,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FB39F2-18C7-4C89-AECD-A2AD62B3166C}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="36.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -16188,7 +16220,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -16208,7 +16240,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -16228,7 +16260,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -16248,7 +16280,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -16268,14 +16300,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="2">
@@ -16288,7 +16320,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -16305,7 +16337,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -16322,7 +16354,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -16339,7 +16371,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -16359,7 +16391,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -16379,7 +16411,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -16396,7 +16428,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -16416,7 +16448,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -16436,7 +16468,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -16456,7 +16488,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -16476,7 +16508,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -16493,7 +16525,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -16513,7 +16545,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -16530,7 +16562,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -16547,7 +16579,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -16567,7 +16599,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -16587,7 +16619,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -16604,7 +16636,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -16621,7 +16653,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -16638,7 +16670,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -16655,7 +16687,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -16672,7 +16704,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -16689,7 +16721,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -16706,7 +16738,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -16723,7 +16755,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -16743,7 +16775,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -16760,7 +16792,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -16777,7 +16809,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -16794,7 +16826,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -16811,7 +16843,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -16828,7 +16860,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>84</v>
       </c>
@@ -16840,7 +16872,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>117</v>
       </c>
@@ -16852,7 +16884,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>117</v>
       </c>
@@ -16864,7 +16896,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>117</v>
       </c>
@@ -16876,7 +16908,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>117</v>
       </c>
@@ -16888,7 +16920,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>117</v>
       </c>
@@ -16900,7 +16932,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>117</v>
       </c>
@@ -16912,7 +16944,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>117</v>
       </c>
@@ -16924,7 +16956,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>117</v>
       </c>
@@ -16936,7 +16968,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>117</v>
       </c>
@@ -16948,7 +16980,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>117</v>
       </c>
@@ -16959,7 +16991,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>156</v>
       </c>
@@ -16980,7 +17012,7 @@
         <v>Gabi (2022.2)_DE: Acrylonitrile-butadiene-styrene (ABS) in waste incineration plant Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>156</v>
       </c>
@@ -17001,7 +17033,7 @@
         <v>Gabi (2022.2)_DE: Polycarbonate (PC) in waste incineration plant Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>156</v>
       </c>
@@ -17022,7 +17054,7 @@
         <v>LCA for experts (2024.1)_DE: Polyethylene (PE) in waste incineration plant (0% H2O content) Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>156</v>
       </c>
@@ -17043,7 +17075,7 @@
         <v>Gabi (2022.2)_DE: Polyethylene terephthalate (PET) in waste incineration plant Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>156</v>
       </c>
@@ -17064,7 +17096,7 @@
         <v>Gabi (2022.2)_DE: Polyamide (PA) 6 in waste incineration plant Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>156</v>
       </c>
@@ -17085,7 +17117,7 @@
         <v>Gabi (2022.2)_DE: Polyamide (PA) 6.6 in waste incineration plant Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>156</v>
       </c>
@@ -17106,7 +17138,7 @@
         <v>Gabi (2022.2)_DE: Polyethylene terephthalate (PET) in waste incineration plant Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>156</v>
       </c>
@@ -17127,7 +17159,7 @@
         <v>Gabi (2022.2)_DE: Polyamide (PA) 6 in waste incineration plant Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>156</v>
       </c>
@@ -17145,7 +17177,7 @@
         <v>Gabi (2022.2)_DE: Polyamide (PA) 6.6 in waste incineration plant Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>156</v>
       </c>
@@ -17166,7 +17198,7 @@
         <v>GaBi (2022.2)_DE: Polyvinyl chloride (PVC) in waste incineration plant; waste-to-energy plant with dry flue gas treatment, without collection, transport and pre-treatment; production mix (region specific plants), at plant; 18.0 MJ/kg net calorific value</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>156</v>
       </c>
@@ -17187,7 +17219,7 @@
         <v>Gabi (2022.2)_DE: Plastics (unspecified) in waste incineration plant Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>156</v>
       </c>
@@ -17208,7 +17240,7 @@
         <v>Gabi (2022.2)_DE: Plastics (unspecified) in waste incineration plant Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>156</v>
       </c>
@@ -17229,7 +17261,7 @@
         <v>LCA for experts (2024.1)_DE: Polypropylene (PP) in waste incineration plant (0% H2O content) Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>156</v>
       </c>
@@ -17250,7 +17282,7 @@
         <v>Gabi (2022.2)_DE: Polystyrene (PS) in waste incineration plant Sphera &lt;t-agg&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>156</v>
       </c>
@@ -17268,7 +17300,7 @@
         <v>Gabi (2022.2)_DE: Polybutadiene (PB) in waste incineration plant Sphera &lt;t-agg&gt;, waste-to-energy plant with dry flue gas treatment, without collection, transport and pre-treatment, production mix (region specific plants), at plant, 41.6 MJ/kg net calorific value</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>156</v>
       </c>
@@ -17289,7 +17321,7 @@
         <v>Gabi (2022.2)_DE: Polymethylmethacrylate (PMMA) in waste incineration plant Sphera &lt;t-agg&gt;, waste-to-energy plant with dry flue gas treatment, without collection, transport and pre-treatment, production mix (region specific plants), at plant, 25.1 MJ/kg net calorific value</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>120</v>
       </c>
@@ -17306,7 +17338,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>120</v>
       </c>
@@ -17323,37 +17355,50 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D66" s="4"/>
+      <c r="C66" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D66" s="8">
+        <v>0.3</v>
+      </c>
       <c r="E66" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D67" s="4"/>
+      <c r="C67" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D67" s="8">
+        <v>1</v>
+      </c>
       <c r="E67" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>120</v>
       </c>
       <c r="B68" t="s">
         <v>123</v>
       </c>
+      <c r="C68" t="s">
+        <v>162</v>
+      </c>
       <c r="D68" s="2">
         <v>0.39970831275007851</v>
       </c>
@@ -17364,13 +17409,16 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>120</v>
       </c>
       <c r="B69" t="s">
         <v>124</v>
       </c>
+      <c r="C69" t="s">
+        <v>163</v>
+      </c>
       <c r="D69" s="2">
         <v>0.24423822562094591</v>
       </c>
@@ -17381,13 +17429,16 @@
         <v>136</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>120</v>
       </c>
       <c r="B70" t="s">
         <v>125</v>
       </c>
+      <c r="C70" t="s">
+        <v>164</v>
+      </c>
       <c r="D70" s="2">
         <v>0.11525018296731784</v>
       </c>
@@ -17398,13 +17449,16 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>120</v>
       </c>
       <c r="B71" t="s">
         <v>126</v>
       </c>
+      <c r="C71" t="s">
+        <v>165</v>
+      </c>
       <c r="D71" s="2">
         <v>6.5184568658291961E-2</v>
       </c>
@@ -17415,13 +17469,16 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>120</v>
       </c>
       <c r="B72" t="s">
         <v>127</v>
       </c>
+      <c r="C72" t="s">
+        <v>166</v>
+      </c>
       <c r="D72" s="2">
         <v>6.0594767899999997E-3</v>
       </c>
@@ -17432,13 +17489,16 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>120</v>
       </c>
       <c r="B73" t="s">
         <v>128</v>
       </c>
+      <c r="C73" t="s">
+        <v>161</v>
+      </c>
       <c r="D73" s="2">
         <v>9.5242999999999994E-3</v>
       </c>
@@ -17449,13 +17509,16 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>120</v>
       </c>
       <c r="B74" t="s">
         <v>129</v>
       </c>
+      <c r="C74" t="s">
+        <v>167</v>
+      </c>
       <c r="D74" s="2">
         <v>3.5394460000000003E-2</v>
       </c>
@@ -17466,13 +17529,16 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>120</v>
       </c>
       <c r="B75" t="s">
         <v>130</v>
       </c>
+      <c r="C75" t="s">
+        <v>168</v>
+      </c>
       <c r="D75" s="2">
         <v>6.5247201979190747E-2</v>
       </c>
@@ -17483,7 +17549,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>144</v>
       </c>
@@ -17503,15 +17569,18 @@
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>147</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>152</v>
       </c>
@@ -17519,7 +17588,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>152</v>
       </c>

</xml_diff>